<commit_message>
Improved point addition algorithm
</commit_message>
<xml_diff>
--- a/doc/OpCounter.xlsx
+++ b/doc/OpCounter.xlsx
@@ -13851,7 +13851,7 @@
         <v>1476</v>
       </c>
       <c r="H1482">
-        <f t="shared" ref="H1482:H1545" si="24">H1480+H1481</f>
+        <f t="shared" ref="H1482" si="24">H1480+H1481</f>
         <v>1.3069892237633987E+308</v>
       </c>
     </row>
@@ -14060,8 +14060,8 @@
         <v>1</v>
       </c>
       <c r="O14">
-        <f>2*F2</f>
-        <v>30</v>
+        <f>F2</f>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="5:19">
@@ -14088,7 +14088,7 @@
         <v>7</v>
       </c>
       <c r="J17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="4:19">
@@ -14144,8 +14144,8 @@
         <v>2</v>
       </c>
       <c r="O21">
-        <f>F2</f>
-        <v>15</v>
+        <f>2*F2</f>
+        <v>30</v>
       </c>
       <c r="Q21">
         <f>6*F3+1</f>
@@ -14166,27 +14166,27 @@
       </c>
       <c r="F23">
         <f ca="1">F7*$F$23+F8*$G$23+F9*$H$23+F10*$I$23+F11*$J$23+F12*$K$23+F13*$L$23+F14*$M$23+F15*$N$23+F16*$O$23+F17*$P$23+F18*$Q$23+F19*$R$23+F20*$S$23+F21</f>
-        <v>391997</v>
+        <v>207777</v>
       </c>
       <c r="G23">
         <f t="shared" ref="G23:S23" ca="1" si="0">G7*$F$23+G8*$G$23+G9*$H$23+G10*$I$23+G11*$J$23+G12*$K$23+G13*$L$23+G14*$M$23+G15*$N$23+G16*$O$23+G17*$P$23+G18*$Q$23+G19*$R$23+G20*$S$23+G21</f>
-        <v>195997</v>
+        <v>103887</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="0"/>
-        <v>99606</v>
+        <v>52796</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="0"/>
-        <v>96392</v>
+        <v>51092</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="0"/>
-        <v>3213</v>
+        <v>1703</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="0"/>
-        <v>3214</v>
+        <v>1704</v>
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="0"/>
@@ -14202,11 +14202,11 @@
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="0"/>
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="P23">
         <f t="shared" ca="1" si="0"/>
-        <v>1330</v>
+        <v>1300</v>
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="0"/>
@@ -14227,27 +14227,27 @@
       </c>
       <c r="F24">
         <f ca="1">F8*$G$24+F9*$H$24+F10*$I$24+F11*$J$24+F12*$K$24+F13*$L$24+F14*$M$24+F15*$N$24+F16*$O$24+F17*$P$24+F18*$Q$24+F19*$R$24+F20*$S$24+1</f>
-        <v>45637</v>
+        <v>21847</v>
       </c>
       <c r="G24">
         <f ca="1">G7*$F$24+G9*$H$24+G10*$I$24+G11*$J$24+G12*$K$24+G13*$L$24+G14*$M$24+G15*$N$24+G16*$O$24+G17*$P$24+G18*$Q$24+G19*$R$24+G20*$S$24+1</f>
-        <v>22817</v>
+        <v>10922</v>
       </c>
       <c r="H24">
         <f ca="1">H7*$F$24+H8*$G$24+H10*$I$24+H11*$J$24+H12*$K$24+H13*$L$24+H14*$M$24+H15*$N$24+H16*$O$24+H17*$P$24+H18*$Q$24+H19*$R$24+H20*$S$24+1</f>
-        <v>11598</v>
+        <v>5553</v>
       </c>
       <c r="I24">
         <f ca="1">I7*$F$24+I8*$G$24+I9*$H$24+I11*$J$24+I12*$K$24+I13*$L$24+I14*$M$24+I15*$N$24+I16*$O$24+I17*$P$24+I18*$Q$24+I19*$R$24+I20*$S$24+1</f>
-        <v>11221</v>
+        <v>5371</v>
       </c>
       <c r="J24">
         <f ca="1">J7*$F$24+J8*$G$24+J9*$H$24+J10*$I$24+J12*$K$24+J13*$L$24+J14*$M$24+J15*$N$24+J16*$O$24+J17*$P$24+J18*$Q$24+J19*$R$24+J20*$S$24+1</f>
-        <v>374</v>
+        <v>179</v>
       </c>
       <c r="K24">
         <f ca="1">K7*$F$24+K8*$G$24+K9*$H$24+K10*$I$24+K11*$J$24+K13*$L$24+K14*$M$24+K15*$N$24+K16*$O$24+K17*$P$24+K18*$Q$24+K19*$R$24+K20*$S$24+1</f>
-        <v>376</v>
+        <v>181</v>
       </c>
       <c r="L24">
         <f ca="1">L7*$F$24+L8*$G$24+L9*$H$24+L10*$I$24+L11*$J$24+L12*$K$24+L14*$M$24+L15*$N$24+L16*$O$24+L17*$P$24+L18*$Q$24+L19*$R$24+L20*$S$24+1</f>
@@ -14263,11 +14263,11 @@
       </c>
       <c r="O24">
         <f ca="1">O7*$F$24+O8*$G$24+O9*$H$24+O10*$I$24+O11*$J$24+O12*$K$24+O13*$L$24+O14*$M$24+O15*$N$24+O17*$P$24+O18*$Q$24+O19*$R$24+O20*$S$24+1</f>
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="P24">
         <f ca="1">P7*$F$24+P8*$G$24+P9*$H$24+P10*$I$24+P11*$J$24+P12*$K$24+P13*$L$24+P14*$M$24+P15*$N$24+P16*$O$24+P18*$Q$24+P19*$R$24+P20*$S$24+1</f>
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="Q24">
         <f ca="1">Q7*$F$24+Q8*$G$24+Q9*$H$24+Q10*$I$24+Q11*$J$24+Q12*$K$24+Q13*$L$24+Q14*$M$24+Q15*$N$24+Q16*$O$24+Q17*$P$24+Q19*$R$24+Q20*$S$24+1</f>

</xml_diff>

<commit_message>
Fully implemented scalar multiplication
</commit_message>
<xml_diff>
--- a/doc/OpCounter.xlsx
+++ b/doc/OpCounter.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>PointMultiplier</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -13862,7 +13865,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D2:S24"/>
+  <dimension ref="D2:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -14083,7 +14086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:19">
+    <row r="17" spans="4:20">
       <c r="E17" s="3" t="s">
         <v>7</v>
       </c>
@@ -14091,7 +14094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="4:19">
+    <row r="18" spans="4:20">
       <c r="E18" s="3" t="s">
         <v>8</v>
       </c>
@@ -14099,7 +14102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="4:19">
+    <row r="19" spans="4:20">
       <c r="E19" s="3" t="s">
         <v>12</v>
       </c>
@@ -14108,7 +14111,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="4:19">
+    <row r="20" spans="4:20">
       <c r="E20" s="3" t="s">
         <v>13</v>
       </c>
@@ -14117,7 +14120,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="4:19">
+    <row r="21" spans="4:20">
       <c r="D21">
         <f>F2</f>
         <v>15</v>
@@ -14159,8 +14162,11 @@
         <f>F2</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="4:19">
+      <c r="T21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="4:20">
       <c r="E23" s="6" t="s">
         <v>19</v>
       </c>
@@ -14221,7 +14227,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="4:19">
+    <row r="24" spans="4:20">
       <c r="E24" s="6" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Extended scalar integer operations to algorithm
</commit_message>
<xml_diff>
--- a/doc/OpCounter.xlsx
+++ b/doc/OpCounter.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>PointMultiplier</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Number</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
 </sst>
 </file>
@@ -13865,7 +13862,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D2:T24"/>
+  <dimension ref="D2:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -14086,7 +14083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:20">
+    <row r="17" spans="4:19">
       <c r="E17" s="3" t="s">
         <v>7</v>
       </c>
@@ -14094,7 +14091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="4:20">
+    <row r="18" spans="4:19">
       <c r="E18" s="3" t="s">
         <v>8</v>
       </c>
@@ -14102,7 +14099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="4:20">
+    <row r="19" spans="4:19">
       <c r="E19" s="3" t="s">
         <v>12</v>
       </c>
@@ -14111,7 +14108,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="4:20">
+    <row r="20" spans="4:19">
       <c r="E20" s="3" t="s">
         <v>13</v>
       </c>
@@ -14120,7 +14117,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="4:20">
+    <row r="21" spans="4:19">
       <c r="D21">
         <f>F2</f>
         <v>15</v>
@@ -14159,40 +14156,37 @@
         <v>15</v>
       </c>
       <c r="S21">
-        <f>F2</f>
-        <v>15</v>
-      </c>
-      <c r="T21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="4:20">
+        <f>(F2+1)*2+3</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="4:19">
       <c r="E23" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F23">
         <f ca="1">F7*$F$23+F8*$G$23+F9*$H$23+F10*$I$23+F11*$J$23+F12*$K$23+F13*$L$23+F14*$M$23+F15*$N$23+F16*$O$23+F17*$P$23+F18*$Q$23+F19*$R$23+F20*$S$23+F21</f>
-        <v>207777</v>
+        <v>266337</v>
       </c>
       <c r="G23">
         <f t="shared" ref="G23:S23" ca="1" si="0">G7*$F$23+G8*$G$23+G9*$H$23+G10*$I$23+G11*$J$23+G12*$K$23+G13*$L$23+G14*$M$23+G15*$N$23+G16*$O$23+G17*$P$23+G18*$Q$23+G19*$R$23+G20*$S$23+G21</f>
-        <v>103887</v>
+        <v>133167</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="0"/>
-        <v>52796</v>
+        <v>67676</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="0"/>
-        <v>51092</v>
+        <v>65492</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="0"/>
-        <v>1703</v>
+        <v>2183</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="0"/>
-        <v>1704</v>
+        <v>2184</v>
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="0"/>
@@ -14212,11 +14206,11 @@
       </c>
       <c r="P23">
         <f t="shared" ca="1" si="0"/>
-        <v>1300</v>
+        <v>1780</v>
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="0"/>
-        <v>1225</v>
+        <v>1705</v>
       </c>
       <c r="R23">
         <f t="shared" ca="1" si="0"/>
@@ -14224,10 +14218,10 @@
       </c>
       <c r="S23">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="4:20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="4:19">
       <c r="E24" s="6" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Creation of even smaller test curve
</commit_message>
<xml_diff>
--- a/doc/OpCounter.xlsx
+++ b/doc/OpCounter.xlsx
@@ -489,7 +489,7 @@
         <v>187</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L10" si="0">2^M4</f>
+        <f t="shared" ref="L4:L18" si="0">2^M4</f>
         <v>3.4028236692093846E+38</v>
       </c>
       <c r="M4">
@@ -624,6 +624,16 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="K12">
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <f>2^M12</f>
+        <v>16</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="7:13">
       <c r="G13">
@@ -633,6 +643,16 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
+      <c r="K13">
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <f>2^M13</f>
+        <v>32</v>
+      </c>
+      <c r="M13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="7:13">
       <c r="G14">
@@ -642,6 +662,16 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
+      <c r="K14">
+        <v>11</v>
+      </c>
+      <c r="L14">
+        <f>2^M14</f>
+        <v>64</v>
+      </c>
+      <c r="M14">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="7:13">
       <c r="G15">
@@ -651,6 +681,16 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
+      <c r="K15">
+        <v>12</v>
+      </c>
+      <c r="L15">
+        <f>2^M15</f>
+        <v>128</v>
+      </c>
+      <c r="M15">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="7:13">
       <c r="G16">
@@ -660,8 +700,18 @@
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="7:8">
+      <c r="K16">
+        <v>14</v>
+      </c>
+      <c r="L16">
+        <f>2^M16</f>
+        <v>256</v>
+      </c>
+      <c r="M16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="7:13">
       <c r="G17">
         <v>11</v>
       </c>
@@ -669,8 +719,18 @@
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="7:8">
+      <c r="K17">
+        <v>15</v>
+      </c>
+      <c r="L17">
+        <f>2^M17</f>
+        <v>512</v>
+      </c>
+      <c r="M17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="7:13">
       <c r="G18">
         <v>12</v>
       </c>
@@ -678,8 +738,18 @@
         <f t="shared" si="1"/>
         <v>144</v>
       </c>
-    </row>
-    <row r="19" spans="7:8">
+      <c r="K18">
+        <v>17</v>
+      </c>
+      <c r="L18">
+        <f>2^M18</f>
+        <v>1024</v>
+      </c>
+      <c r="M18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="7:13">
       <c r="G19">
         <v>13</v>
       </c>
@@ -688,7 +758,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="7:8">
+    <row r="20" spans="7:13">
       <c r="G20">
         <v>14</v>
       </c>
@@ -697,7 +767,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="21" spans="7:8">
+    <row r="21" spans="7:13">
       <c r="G21">
         <v>15</v>
       </c>
@@ -706,7 +776,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="22" spans="7:8">
+    <row r="22" spans="7:13">
       <c r="G22">
         <v>16</v>
       </c>
@@ -715,7 +785,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="23" spans="7:8">
+    <row r="23" spans="7:13">
       <c r="G23">
         <v>17</v>
       </c>
@@ -724,7 +794,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="24" spans="7:8">
+    <row r="24" spans="7:13">
       <c r="G24">
         <v>18</v>
       </c>
@@ -733,7 +803,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="25" spans="7:8">
+    <row r="25" spans="7:13">
       <c r="G25">
         <v>19</v>
       </c>
@@ -742,7 +812,7 @@
         <v>4181</v>
       </c>
     </row>
-    <row r="26" spans="7:8">
+    <row r="26" spans="7:13">
       <c r="G26">
         <v>20</v>
       </c>
@@ -751,7 +821,7 @@
         <v>6765</v>
       </c>
     </row>
-    <row r="27" spans="7:8">
+    <row r="27" spans="7:13">
       <c r="G27">
         <v>21</v>
       </c>
@@ -760,7 +830,7 @@
         <v>10946</v>
       </c>
     </row>
-    <row r="28" spans="7:8">
+    <row r="28" spans="7:13">
       <c r="G28">
         <v>22</v>
       </c>
@@ -769,7 +839,7 @@
         <v>17711</v>
       </c>
     </row>
-    <row r="29" spans="7:8">
+    <row r="29" spans="7:13">
       <c r="G29">
         <v>23</v>
       </c>
@@ -778,7 +848,7 @@
         <v>28657</v>
       </c>
     </row>
-    <row r="30" spans="7:8">
+    <row r="30" spans="7:13">
       <c r="G30" s="1">
         <v>24</v>
       </c>
@@ -787,7 +857,7 @@
         <v>46368</v>
       </c>
     </row>
-    <row r="31" spans="7:8">
+    <row r="31" spans="7:13">
       <c r="G31">
         <v>25</v>
       </c>
@@ -796,7 +866,7 @@
         <v>75025</v>
       </c>
     </row>
-    <row r="32" spans="7:8">
+    <row r="32" spans="7:13">
       <c r="G32">
         <v>26</v>
       </c>
@@ -13864,7 +13934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -13877,7 +13949,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="7">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I2">
         <v>15</v>
@@ -13909,7 +13981,7 @@
         <v>14</v>
       </c>
       <c r="F3" s="7">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="I3">
         <v>24</v>
@@ -14027,7 +14099,7 @@
       </c>
       <c r="I11">
         <f>2*F2</f>
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -14061,7 +14133,7 @@
       </c>
       <c r="O14">
         <f>F2</f>
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="5:19">
@@ -14105,7 +14177,7 @@
       </c>
       <c r="Q19">
         <f>2*F3</f>
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="4:19">
@@ -14114,13 +14186,13 @@
       </c>
       <c r="Q20">
         <f>F3</f>
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="4:19">
       <c r="D21">
         <f>F2</f>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>15</v>
@@ -14145,19 +14217,19 @@
       </c>
       <c r="O21">
         <f>2*F2</f>
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="Q21">
         <f>6*F3+1</f>
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="R21">
         <f>F2</f>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="S21">
         <f>(F2+1)*2+3</f>
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="4:19">
@@ -14166,27 +14238,27 @@
       </c>
       <c r="F23">
         <f ca="1">F7*$F$23+F8*$G$23+F9*$H$23+F10*$I$23+F11*$J$23+F12*$K$23+F13*$L$23+F14*$M$23+F15*$N$23+F16*$O$23+F17*$P$23+F18*$Q$23+F19*$R$23+F20*$S$23+F21</f>
-        <v>266337</v>
+        <v>29711</v>
       </c>
       <c r="G23">
         <f t="shared" ref="G23:S23" ca="1" si="0">G7*$F$23+G8*$G$23+G9*$H$23+G10*$I$23+G11*$J$23+G12*$K$23+G13*$L$23+G14*$M$23+G15*$N$23+G16*$O$23+G17*$P$23+G18*$Q$23+G19*$R$23+G20*$S$23+G21</f>
-        <v>133167</v>
+        <v>14854</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="0"/>
-        <v>67676</v>
+        <v>7725</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="0"/>
-        <v>65492</v>
+        <v>7130</v>
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="0"/>
-        <v>2183</v>
+        <v>594</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="0"/>
-        <v>2184</v>
+        <v>595</v>
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="0"/>
@@ -14202,23 +14274,23 @@
       </c>
       <c r="O23">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="P23">
         <f t="shared" ca="1" si="0"/>
-        <v>1780</v>
+        <v>416</v>
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="0"/>
-        <v>1705</v>
+        <v>386</v>
       </c>
       <c r="R23">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="S23">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="4:19">
@@ -14227,27 +14299,27 @@
       </c>
       <c r="F24">
         <f ca="1">F8*$G$24+F9*$H$24+F10*$I$24+F11*$J$24+F12*$K$24+F13*$L$24+F14*$M$24+F15*$N$24+F16*$O$24+F17*$P$24+F18*$Q$24+F19*$R$24+F20*$S$24+1</f>
-        <v>21847</v>
+        <v>4309</v>
       </c>
       <c r="G24">
         <f ca="1">G7*$F$24+G9*$H$24+G10*$I$24+G11*$J$24+G12*$K$24+G13*$L$24+G14*$M$24+G15*$N$24+G16*$O$24+G17*$P$24+G18*$Q$24+G19*$R$24+G20*$S$24+1</f>
-        <v>10922</v>
+        <v>2153</v>
       </c>
       <c r="H24">
         <f ca="1">H7*$F$24+H8*$G$24+H10*$I$24+H11*$J$24+H12*$K$24+H13*$L$24+H14*$M$24+H15*$N$24+H16*$O$24+H17*$P$24+H18*$Q$24+H19*$R$24+H20*$S$24+1</f>
-        <v>5553</v>
+        <v>1122</v>
       </c>
       <c r="I24">
         <f ca="1">I7*$F$24+I8*$G$24+I9*$H$24+I11*$J$24+I12*$K$24+I13*$L$24+I14*$M$24+I15*$N$24+I16*$O$24+I17*$P$24+I18*$Q$24+I19*$R$24+I20*$S$24+1</f>
-        <v>5371</v>
+        <v>1033</v>
       </c>
       <c r="J24">
         <f ca="1">J7*$F$24+J8*$G$24+J9*$H$24+J10*$I$24+J12*$K$24+J13*$L$24+J14*$M$24+J15*$N$24+J16*$O$24+J17*$P$24+J18*$Q$24+J19*$R$24+J20*$S$24+1</f>
-        <v>179</v>
+        <v>86</v>
       </c>
       <c r="K24">
         <f ca="1">K7*$F$24+K8*$G$24+K9*$H$24+K10*$I$24+K11*$J$24+K13*$L$24+K14*$M$24+K15*$N$24+K16*$O$24+K17*$P$24+K18*$Q$24+K19*$R$24+K20*$S$24+1</f>
-        <v>181</v>
+        <v>88</v>
       </c>
       <c r="L24">
         <f ca="1">L7*$F$24+L8*$G$24+L9*$H$24+L10*$I$24+L11*$J$24+L12*$K$24+L14*$M$24+L15*$N$24+L16*$O$24+L17*$P$24+L18*$Q$24+L19*$R$24+L20*$S$24+1</f>
@@ -14263,15 +14335,15 @@
       </c>
       <c r="O24">
         <f ca="1">O7*$F$24+O8*$G$24+O9*$H$24+O10*$I$24+O11*$J$24+O12*$K$24+O13*$L$24+O14*$M$24+O15*$N$24+O17*$P$24+O18*$Q$24+O19*$R$24+O20*$S$24+1</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="P24">
         <f ca="1">P7*$F$24+P8*$G$24+P9*$H$24+P10*$I$24+P11*$J$24+P12*$K$24+P13*$L$24+P14*$M$24+P15*$N$24+P16*$O$24+P18*$Q$24+P19*$R$24+P20*$S$24+1</f>
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="Q24">
         <f ca="1">Q7*$F$24+Q8*$G$24+Q9*$H$24+Q10*$I$24+Q11*$J$24+Q12*$K$24+Q13*$L$24+Q14*$M$24+Q15*$N$24+Q16*$O$24+Q17*$P$24+Q19*$R$24+Q20*$S$24+1</f>
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="R24">
         <f ca="1">R7*$F$24+R8*$G$24+R9*$H$24+R10*$I$24+R11*$J$24+R12*$K$24+R13*$L$24+R14*$M$24+R15*$N$24+R16*$O$24+R17*$P$24+R18*$Q$24+R20*$S$24+1</f>

</xml_diff>